<commit_message>
Code Progress - additional java code
Update: All 8 java classes were added under "Java Code - used in jars"
Directory
</commit_message>
<xml_diff>
--- a/public_html/tool/uploads/SJO Millennium and Sierra (III) Delivered Files List.xlsx
+++ b/public_html/tool/uploads/SJO Millennium and Sierra (III) Delivered Files List.xlsx
@@ -14,12 +14,12 @@
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="46">
   <si>
     <t>Latin-1</t>
   </si>
@@ -33,9 +33,6 @@
     <t>Courses</t>
   </si>
   <si>
-    <t>Order Payments</t>
-  </si>
-  <si>
     <t>Open Orders</t>
   </si>
   <si>
@@ -147,49 +144,19 @@
     <t>sjsu_p2e_12082015.csv</t>
   </si>
   <si>
-    <t>sjsu_bibs_01_12062015.mrc</t>
-  </si>
-  <si>
-    <t>sjsu_bibs_02_12062015.mrc</t>
-  </si>
-  <si>
-    <t>sjsu_bibs_03_12062015.mrc</t>
-  </si>
-  <si>
-    <t>sjsu_bibs_04_12062015.mrc</t>
-  </si>
-  <si>
-    <t>sjsu_bibs_05_12062015.mrc</t>
-  </si>
-  <si>
-    <t>sjsu_bibs_06_12062015.mrc</t>
-  </si>
-  <si>
-    <t>sjsu_bibs_07_12062015.mrc</t>
-  </si>
-  <si>
-    <t>sjsu_bibs_08_12062015.mrc</t>
-  </si>
-  <si>
-    <t>sjsu_bibs_09_12062015.mrc</t>
-  </si>
-  <si>
-    <t>sjsu_items_2_12032015.csv</t>
-  </si>
-  <si>
-    <t>sjsu_items_1_12032015.csv</t>
-  </si>
-  <si>
-    <t>sjsu_items_3_12032015.csv</t>
-  </si>
-  <si>
     <t>sjsu_orders_a_12032015.csv</t>
   </si>
   <si>
     <t>sjsu_orders_b_12032015.csv</t>
   </si>
   <si>
-    <t>sjsu_bibs_10_12112015.mrc</t>
+    <t>sjsu_bibs_01_12062015.mrc,sjsu_bibs_02_12062015.mrc,sjsu_bibs_03_12062015.mrc,sjsu_bibs_04_12062015.mrc,sjsu_bibs_05_12062015.mrc,sjsu_bibs_06_12062015.mrc,sjsu_bibs_07_12062015.mrc,sjsu_bibs_08_12062015.mrc,sjsu_bibs_09_12062015.mrc,sjsu_bibs_10_12112015.mrc</t>
+  </si>
+  <si>
+    <t>sjsu_items_1_12032015.csv,sjsu_items_2_12032015.csv,sjsu_items_3_12032015.csv</t>
+  </si>
+  <si>
+    <t>Payments</t>
   </si>
 </sst>
 </file>
@@ -274,7 +241,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -331,6 +298,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -638,49 +611,50 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H39"/>
+  <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="36.875" customWidth="1"/>
+    <col min="1" max="1" width="27.75" customWidth="1"/>
     <col min="2" max="2" width="15.875" customWidth="1"/>
     <col min="3" max="3" width="31.125" customWidth="1"/>
-    <col min="4" max="4" width="30.625" customWidth="1"/>
-    <col min="5" max="5" width="28.625" customWidth="1"/>
-    <col min="6" max="7" width="22.5" customWidth="1"/>
+    <col min="4" max="4" width="22.75" customWidth="1"/>
+    <col min="5" max="5" width="17.5" customWidth="1"/>
+    <col min="6" max="6" width="19.5" customWidth="1"/>
+    <col min="7" max="7" width="15.125" customWidth="1"/>
     <col min="8" max="8" width="34.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:8" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:8" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:8" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -688,612 +662,392 @@
     </row>
     <row r="7" spans="1:8" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
     <row r="9" spans="1:8" s="8" customFormat="1" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D9" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="E9" s="10" t="s">
-        <v>31</v>
-      </c>
       <c r="F9" s="10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G9" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H9" s="9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="126.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D10" s="19">
         <v>20151210</v>
       </c>
-      <c r="E10" s="1">
-        <v>184526</v>
-      </c>
-      <c r="F10" s="23">
-        <v>150000</v>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1">
+        <v>1284899</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H10" s="1"/>
+        <v>14</v>
+      </c>
+      <c r="H10" s="25"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="1"/>
-      <c r="B11" s="2"/>
+      <c r="A11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="C11" s="1" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="D11" s="19">
-        <v>20151210</v>
-      </c>
-      <c r="E11" s="1">
-        <v>172168</v>
-      </c>
-      <c r="F11" s="23">
-        <v>150000</v>
-      </c>
-      <c r="G11" s="1"/>
+        <v>20151201</v>
+      </c>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14">
+        <v>8371</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="H11" s="1"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="1"/>
-      <c r="B12" s="2"/>
+    <row r="12" spans="1:8" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="C12" s="1" t="s">
         <v>44</v>
       </c>
       <c r="D12" s="19">
-        <v>20151210</v>
-      </c>
-      <c r="E12" s="1">
-        <v>163866</v>
-      </c>
-      <c r="F12" s="23">
-        <v>150000</v>
-      </c>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
+        <v>20151203</v>
+      </c>
+      <c r="E12" s="16"/>
+      <c r="F12" s="16">
+        <v>1382738</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H12" s="24"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="1"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="1" t="s">
+      <c r="A13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="1"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H13" s="1"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="1"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H14" s="1"/>
+    </row>
+    <row r="15" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" s="1"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H15" s="1"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" t="s">
+        <v>33</v>
+      </c>
+      <c r="D16" s="20">
+        <v>20151201</v>
+      </c>
+      <c r="E16" s="15"/>
+      <c r="F16" s="15">
+        <v>44318</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" s="19">
+        <v>20151201</v>
+      </c>
+      <c r="E17" s="16"/>
+      <c r="F17" s="16">
+        <v>19301</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H17" s="1"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D18" s="19">
+        <v>20151201</v>
+      </c>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14">
+        <v>401</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H18" s="1"/>
+    </row>
+    <row r="19" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D19" s="21">
+        <v>20151201</v>
+      </c>
+      <c r="E19" s="17"/>
+      <c r="F19" s="17">
+        <v>494</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="H19" s="6"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D20" s="22">
+        <v>20151203</v>
+      </c>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13">
+        <v>740</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="H20" s="3"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D21" s="22">
+        <v>20151203</v>
+      </c>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13">
+        <v>1593</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="H21" s="3"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" s="3"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D22" s="22">
+        <v>20151203</v>
+      </c>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13">
+        <v>1593</v>
+      </c>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="D13" s="19">
-        <v>20151210</v>
-      </c>
-      <c r="E13" s="1">
-        <v>201355</v>
-      </c>
-      <c r="F13" s="23">
-        <v>150000</v>
-      </c>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="1"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D14" s="19">
-        <v>20151210</v>
-      </c>
-      <c r="E14" s="1">
-        <v>214132</v>
-      </c>
-      <c r="F14" s="23">
-        <v>150000</v>
-      </c>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="1"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D15" s="19">
-        <v>20151210</v>
-      </c>
-      <c r="E15" s="1">
-        <v>227203</v>
-      </c>
-      <c r="F15" s="23">
-        <v>150000</v>
-      </c>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="1"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D16" s="19">
-        <v>20151210</v>
-      </c>
-      <c r="E16" s="1">
-        <v>244915</v>
-      </c>
-      <c r="F16" s="23">
-        <v>150000</v>
-      </c>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A17" s="1"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D17" s="19">
-        <v>20151210</v>
-      </c>
-      <c r="E17" s="1">
-        <v>143776</v>
-      </c>
-      <c r="F17" s="23">
-        <v>69317</v>
-      </c>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A18" s="1"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D18" s="19">
-        <v>20151210</v>
-      </c>
-      <c r="E18" s="1">
-        <v>18765</v>
-      </c>
-      <c r="F18" s="23">
-        <v>7795</v>
-      </c>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A19" s="1"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D19" s="19">
-        <v>20151211</v>
-      </c>
-      <c r="E19" s="1">
-        <v>292546</v>
-      </c>
-      <c r="F19" s="23">
-        <v>157787</v>
-      </c>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B20" s="2" t="s">
+      <c r="B23" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D20" s="19">
-        <v>20151201</v>
-      </c>
-      <c r="E20" s="14">
-        <v>90</v>
-      </c>
-      <c r="F20" s="14">
-        <v>8371</v>
-      </c>
-      <c r="G20" s="1" t="s">
+      <c r="C23" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D23" s="22">
+        <v>20151204</v>
+      </c>
+      <c r="E23" s="3"/>
+      <c r="F23" s="13">
+        <v>398</v>
+      </c>
+      <c r="G23" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="H20" s="1"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D21" s="19">
-        <v>20151203</v>
-      </c>
-      <c r="E21" s="16">
-        <v>138416</v>
-      </c>
-      <c r="F21" s="16">
-        <v>500000</v>
-      </c>
-      <c r="G21" s="1" t="s">
+      <c r="H23" s="3"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="H21" s="1"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A22" s="1"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D22" s="19">
-        <v>20151203</v>
-      </c>
-      <c r="E22" s="16">
-        <v>135721</v>
-      </c>
-      <c r="F22" s="16">
-        <v>499998</v>
-      </c>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A23" s="1"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D23" s="19">
-        <v>20151203</v>
-      </c>
-      <c r="E23" s="16">
-        <v>84222</v>
-      </c>
-      <c r="F23" s="16">
-        <v>382740</v>
-      </c>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A24" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C24" s="1"/>
-      <c r="D24" s="19"/>
-      <c r="E24" s="14"/>
-      <c r="F24" s="14"/>
-      <c r="G24" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="H24" s="1"/>
+      <c r="H24" s="3"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>28</v>
+        <v>2</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C25" s="1"/>
-      <c r="D25" s="19"/>
-      <c r="E25" s="14"/>
-      <c r="F25" s="14"/>
+        <v>1</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D25" s="1">
+        <v>20151208</v>
+      </c>
+      <c r="E25" s="23">
+        <v>4716</v>
+      </c>
+      <c r="F25" s="14">
+        <v>229967</v>
+      </c>
       <c r="G25" s="1" t="s">
         <v>0</v>
       </c>
       <c r="H25" s="1"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
       <c r="C26" s="1"/>
-      <c r="D26" s="19"/>
-      <c r="E26" s="14"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
       <c r="F26" s="14"/>
-      <c r="G26" s="1" t="s">
-        <v>15</v>
-      </c>
+      <c r="G26" s="1"/>
       <c r="H26" s="1"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A27" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C27" t="s">
-        <v>34</v>
-      </c>
-      <c r="D27" s="20">
-        <v>20151201</v>
-      </c>
-      <c r="E27" s="15">
-        <v>11541</v>
-      </c>
-      <c r="F27" s="15">
-        <v>44318</v>
-      </c>
-      <c r="G27" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="14"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A28" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D28" s="19">
-        <v>20151201</v>
-      </c>
-      <c r="E28" s="16">
-        <v>1653</v>
-      </c>
-      <c r="F28" s="16">
-        <v>19301</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="H28" s="1"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A29" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D29" s="19">
-        <v>20151201</v>
-      </c>
-      <c r="E29" s="14">
-        <v>51</v>
-      </c>
-      <c r="F29" s="14">
-        <v>401</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="H29" s="1"/>
-    </row>
-    <row r="30" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B30" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C30" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="D30" s="21">
-        <v>20151201</v>
-      </c>
-      <c r="E30" s="17">
-        <v>97</v>
-      </c>
-      <c r="F30" s="17">
-        <v>494</v>
-      </c>
-      <c r="G30" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="H30" s="6"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A31" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D31" s="22">
-        <v>20151203</v>
-      </c>
-      <c r="E31" s="13">
-        <v>51</v>
-      </c>
-      <c r="F31" s="13">
-        <v>740</v>
-      </c>
-      <c r="G31" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="H31" s="3"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A32" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="D32" s="22">
-        <v>20151203</v>
-      </c>
-      <c r="E32" s="13">
-        <v>1164</v>
-      </c>
-      <c r="F32" s="13">
-        <v>1593</v>
-      </c>
-      <c r="G32" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="H32" s="3"/>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A33" s="3"/>
-      <c r="B33" s="4"/>
-      <c r="C33" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D33" s="22">
-        <v>20151203</v>
-      </c>
-      <c r="E33" s="13">
-        <v>844</v>
-      </c>
-      <c r="F33" s="13">
-        <v>1593</v>
-      </c>
-      <c r="G33" s="3"/>
-      <c r="H33" s="3"/>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A34" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B34" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D34" s="22">
-        <v>20151204</v>
-      </c>
-      <c r="E34" s="3">
-        <v>55</v>
-      </c>
-      <c r="F34" s="13">
-        <v>398</v>
-      </c>
-      <c r="G34" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="H34" s="3"/>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A35" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C35" s="3"/>
-      <c r="D35" s="3"/>
-      <c r="E35" s="3"/>
-      <c r="F35" s="13"/>
-      <c r="G35" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="H35" s="3"/>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A36" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D36" s="1">
-        <v>20151208</v>
-      </c>
-      <c r="E36" s="23">
-        <v>4716</v>
-      </c>
-      <c r="F36" s="14">
-        <v>229967</v>
-      </c>
-      <c r="G36" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="H36" s="1"/>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A37" s="1"/>
-      <c r="B37" s="1"/>
-      <c r="C37" s="1"/>
-      <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
-      <c r="F37" s="14"/>
-      <c r="G37" s="1"/>
-      <c r="H37" s="1"/>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C38" s="1"/>
-      <c r="D38" s="1"/>
-      <c r="E38" s="1"/>
-      <c r="F38" s="14"/>
-      <c r="G38" s="1"/>
-      <c r="H38" s="1"/>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="F39" s="18"/>
+      <c r="F28" s="18"/>
     </row>
   </sheetData>
   <dataValidations count="4">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4">
       <formula1>"Test, Cutover"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G20:G36">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G10">
+      <formula1>"UTF-8, Ansel"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G11:G25">
       <formula1>"UTF-8, Latin-1"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G10:G19">
-      <formula1>"UTF-8, Ansel"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B10:B36">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B10:B25">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1303,6 +1057,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="External Document" ma:contentTypeID="0x010100D21F5325077A3040AF71719A18A5123600347BF9C197B2B8459A09E01A06CC79AC" ma:contentTypeVersion="2" ma:contentTypeDescription="" ma:contentTypeScope="" ma:versionID="5f8365d3f1c632e05daf43eddb83a028">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="0fa2fffc-844c-4eb5-bf9b-0198ba866acd" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="32d72b4aa68a7008db2176e90a0754ce" ns2:_="">
     <xsd:import namespace="0fa2fffc-844c-4eb5-bf9b-0198ba866acd"/>
@@ -1400,15 +1163,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
   <documentManagement>
@@ -1423,6 +1177,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1F3F1D5C-8813-428F-B184-51DEB994E8F1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8324D054-419F-4625-87C9-E808270FE481}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1435,14 +1197,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1F3F1D5C-8813-428F-B184-51DEB994E8F1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>